<commit_message>
use activities instead of updates
</commit_message>
<xml_diff>
--- a/pipeline.xlsx
+++ b/pipeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gjung18/Workspace/emd/emd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C38E0E-7E9B-F64B-A5BE-0EF038611D2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3311DA37-2693-F146-BD7D-D472F46B0EE0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="30500" windowHeight="16920" activeTab="1" xr2:uid="{95744BB1-B1C7-41ED-B352-8C3E88B99EF1}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Meeting:</t>
   </si>
@@ -164,6 +164,21 @@
   </si>
   <si>
     <t>beta.SAM.gov Link:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Subject:</t>
+  </si>
+  <si>
+    <t>Comments:</t>
+  </si>
+  <si>
+    <t>Status:</t>
+  </si>
+  <si>
+    <t>Last Modified By:</t>
+  </si>
+  <si>
+    <t>Last Modified Date:</t>
   </si>
 </sst>
 </file>
@@ -209,7 +224,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -269,11 +284,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -307,15 +364,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -636,7 +701,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="H1" sqref="H1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1014,10 +1079,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1025,18 +1090,20 @@
     <col min="1" max="1" width="23.1640625" customWidth="1"/>
     <col min="2" max="2" width="52" customWidth="1"/>
     <col min="3" max="3" width="29.1640625" customWidth="1"/>
-    <col min="4" max="4" width="54.5" customWidth="1"/>
+    <col min="4" max="4" width="32.5" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -1044,9 +1111,10 @@
       <c r="C2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D2" s="19"/>
+      <c r="E2" s="20"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
@@ -1054,51 +1122,57 @@
       <c r="C3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D3" s="19"/>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" s="19"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="20"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="19"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="20"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="19"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="20"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="19"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="20"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="3" t="s">
+      <c r="B8" s="17"/>
+      <c r="C8" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D8" s="19"/>
+      <c r="E8" s="20"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
@@ -1106,9 +1180,10 @@
       <c r="C9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D9" s="19"/>
+      <c r="E9" s="20"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
@@ -1116,9 +1191,10 @@
       <c r="C10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D10" s="19"/>
+      <c r="E10" s="20"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
@@ -1126,9 +1202,10 @@
       <c r="C11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D11" s="19"/>
+      <c r="E11" s="20"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>33</v>
       </c>
@@ -1136,9 +1213,10 @@
       <c r="C12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D12" s="19"/>
+      <c r="E12" s="20"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>25</v>
       </c>
@@ -1146,9 +1224,10 @@
       <c r="C13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D13" s="19"/>
+      <c r="E13" s="20"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
@@ -1156,9 +1235,10 @@
       <c r="C14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D14" s="19"/>
+      <c r="E14" s="20"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>38</v>
       </c>
@@ -1166,33 +1246,64 @@
       <c r="C15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D15" s="19"/>
+      <c r="E15" s="20"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="13" t="s">
+      <c r="B16" s="19"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="20"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B16:D16"/>
+  <dataConsolidate/>
+  <mergeCells count="17">
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="77" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>